<commit_message>
single agent data plotting done
</commit_message>
<xml_diff>
--- a/data/OutputFile2.xlsx
+++ b/data/OutputFile2.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M8"/>
+  <dimension ref="A1:M37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -489,11 +489,6 @@
           <t>Nov</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>Dec</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
@@ -534,9 +529,6 @@
       <c r="L2" t="n">
         <v>12</v>
       </c>
-      <c r="M2" t="n">
-        <v>3</v>
-      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -577,9 +569,6 @@
       <c r="L3" t="n">
         <v>9</v>
       </c>
-      <c r="M3" t="n">
-        <v>3</v>
-      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
@@ -620,9 +609,6 @@
       <c r="L4" t="n">
         <v>8</v>
       </c>
-      <c r="M4" t="n">
-        <v>3</v>
-      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
@@ -663,9 +649,6 @@
       <c r="L5" t="n">
         <v>12</v>
       </c>
-      <c r="M5" t="n">
-        <v>3</v>
-      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
@@ -706,9 +689,6 @@
       <c r="L6" t="n">
         <v>12</v>
       </c>
-      <c r="M6" t="n">
-        <v>3</v>
-      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
@@ -749,9 +729,6 @@
       <c r="L7" t="n">
         <v>12</v>
       </c>
-      <c r="M7" t="n">
-        <v>3</v>
-      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
@@ -792,8 +769,594 @@
       <c r="L8" t="n">
         <v>10</v>
       </c>
-      <c r="M8" t="n">
-        <v>3</v>
+    </row>
+    <row r="13">
+      <c r="B13" s="1" t="inlineStr">
+        <is>
+          <t>Jan</t>
+        </is>
+      </c>
+      <c r="C13" s="1" t="inlineStr">
+        <is>
+          <t>Feb</t>
+        </is>
+      </c>
+      <c r="D13" s="1" t="inlineStr">
+        <is>
+          <t>Mar</t>
+        </is>
+      </c>
+      <c r="E13" s="1" t="inlineStr">
+        <is>
+          <t>Apr</t>
+        </is>
+      </c>
+      <c r="F13" s="1" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="G13" s="1" t="inlineStr">
+        <is>
+          <t>Jun</t>
+        </is>
+      </c>
+      <c r="H13" s="1" t="inlineStr">
+        <is>
+          <t>Jul</t>
+        </is>
+      </c>
+      <c r="I13" s="1" t="inlineStr">
+        <is>
+          <t>Aug</t>
+        </is>
+      </c>
+      <c r="J13" s="1" t="inlineStr">
+        <is>
+          <t>Sep</t>
+        </is>
+      </c>
+      <c r="K13" s="1" t="inlineStr">
+        <is>
+          <t>Oct</t>
+        </is>
+      </c>
+      <c r="L13" s="1" t="inlineStr">
+        <is>
+          <t>Nov</t>
+        </is>
+      </c>
+      <c r="M13" s="1" t="inlineStr">
+        <is>
+          <t>avg</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="inlineStr">
+        <is>
+          <t>Verbal Excellence</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>69</v>
+      </c>
+      <c r="C14" t="n">
+        <v>92</v>
+      </c>
+      <c r="D14" t="n">
+        <v>73</v>
+      </c>
+      <c r="E14" t="n">
+        <v>75</v>
+      </c>
+      <c r="F14" t="n">
+        <v>55</v>
+      </c>
+      <c r="G14" t="n">
+        <v>93</v>
+      </c>
+      <c r="H14" t="n">
+        <v>85</v>
+      </c>
+      <c r="I14" t="n">
+        <v>82</v>
+      </c>
+      <c r="J14" t="n">
+        <v>62</v>
+      </c>
+      <c r="K14" t="n">
+        <v>75</v>
+      </c>
+      <c r="L14" t="n">
+        <v>75</v>
+      </c>
+      <c r="M14" t="n">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="inlineStr">
+        <is>
+          <t>Avoid Rude/Unprofessional Behavior/Approach (ARU)</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>100</v>
+      </c>
+      <c r="C15" t="n">
+        <v>100</v>
+      </c>
+      <c r="D15" t="n">
+        <v>100</v>
+      </c>
+      <c r="E15" t="n">
+        <v>100</v>
+      </c>
+      <c r="F15" t="n">
+        <v>100</v>
+      </c>
+      <c r="G15" t="n">
+        <v>93</v>
+      </c>
+      <c r="H15" t="n">
+        <v>92</v>
+      </c>
+      <c r="I15" t="n">
+        <v>100</v>
+      </c>
+      <c r="J15" t="n">
+        <v>100</v>
+      </c>
+      <c r="K15" t="n">
+        <v>100</v>
+      </c>
+      <c r="L15" t="n">
+        <v>100</v>
+      </c>
+      <c r="M15" t="n">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="M16" t="n">
+        <v>87.5</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="M17" t="n">
+        <v>4.38</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="B20" s="1" t="inlineStr">
+        <is>
+          <t>Jan</t>
+        </is>
+      </c>
+      <c r="C20" s="1" t="inlineStr">
+        <is>
+          <t>Feb</t>
+        </is>
+      </c>
+      <c r="D20" s="1" t="inlineStr">
+        <is>
+          <t>Mar</t>
+        </is>
+      </c>
+      <c r="E20" s="1" t="inlineStr">
+        <is>
+          <t>Apr</t>
+        </is>
+      </c>
+      <c r="F20" s="1" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="G20" s="1" t="inlineStr">
+        <is>
+          <t>Jun</t>
+        </is>
+      </c>
+      <c r="H20" s="1" t="inlineStr">
+        <is>
+          <t>Jul</t>
+        </is>
+      </c>
+      <c r="I20" s="1" t="inlineStr">
+        <is>
+          <t>Aug</t>
+        </is>
+      </c>
+      <c r="J20" s="1" t="inlineStr">
+        <is>
+          <t>Sep</t>
+        </is>
+      </c>
+      <c r="K20" s="1" t="inlineStr">
+        <is>
+          <t>Oct</t>
+        </is>
+      </c>
+      <c r="L20" s="1" t="inlineStr">
+        <is>
+          <t>Nov</t>
+        </is>
+      </c>
+      <c r="M20" s="1" t="inlineStr">
+        <is>
+          <t>avg</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="inlineStr">
+        <is>
+          <t>Courteous Approach</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>69</v>
+      </c>
+      <c r="C21" t="n">
+        <v>92</v>
+      </c>
+      <c r="D21" t="n">
+        <v>100</v>
+      </c>
+      <c r="E21" t="n">
+        <v>92</v>
+      </c>
+      <c r="F21" t="n">
+        <v>82</v>
+      </c>
+      <c r="G21" t="n">
+        <v>93</v>
+      </c>
+      <c r="H21" t="n">
+        <v>85</v>
+      </c>
+      <c r="I21" t="n">
+        <v>91</v>
+      </c>
+      <c r="J21" t="n">
+        <v>69</v>
+      </c>
+      <c r="K21" t="n">
+        <v>75</v>
+      </c>
+      <c r="L21" t="n">
+        <v>67</v>
+      </c>
+      <c r="M21" t="n">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="inlineStr">
+        <is>
+          <t>Active Listening</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>100</v>
+      </c>
+      <c r="C22" t="n">
+        <v>100</v>
+      </c>
+      <c r="D22" t="n">
+        <v>100</v>
+      </c>
+      <c r="E22" t="n">
+        <v>100</v>
+      </c>
+      <c r="F22" t="n">
+        <v>100</v>
+      </c>
+      <c r="G22" t="n">
+        <v>93</v>
+      </c>
+      <c r="H22" t="n">
+        <v>100</v>
+      </c>
+      <c r="I22" t="n">
+        <v>100</v>
+      </c>
+      <c r="J22" t="n">
+        <v>100</v>
+      </c>
+      <c r="K22" t="n">
+        <v>92</v>
+      </c>
+      <c r="L22" t="n">
+        <v>100</v>
+      </c>
+      <c r="M22" t="n">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="M23" t="n">
+        <v>91.5</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="M24" t="n">
+        <v>4.58</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="B27" s="1" t="inlineStr">
+        <is>
+          <t>Jan</t>
+        </is>
+      </c>
+      <c r="C27" s="1" t="inlineStr">
+        <is>
+          <t>Feb</t>
+        </is>
+      </c>
+      <c r="D27" s="1" t="inlineStr">
+        <is>
+          <t>Mar</t>
+        </is>
+      </c>
+      <c r="E27" s="1" t="inlineStr">
+        <is>
+          <t>Apr</t>
+        </is>
+      </c>
+      <c r="F27" s="1" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="G27" s="1" t="inlineStr">
+        <is>
+          <t>Jun</t>
+        </is>
+      </c>
+      <c r="H27" s="1" t="inlineStr">
+        <is>
+          <t>Jul</t>
+        </is>
+      </c>
+      <c r="I27" s="1" t="inlineStr">
+        <is>
+          <t>Aug</t>
+        </is>
+      </c>
+      <c r="J27" s="1" t="inlineStr">
+        <is>
+          <t>Sep</t>
+        </is>
+      </c>
+      <c r="K27" s="1" t="inlineStr">
+        <is>
+          <t>Oct</t>
+        </is>
+      </c>
+      <c r="L27" s="1" t="inlineStr">
+        <is>
+          <t>Nov</t>
+        </is>
+      </c>
+      <c r="M27" s="1" t="inlineStr">
+        <is>
+          <t>avg</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="inlineStr">
+        <is>
+          <t>Correct &amp; Complete Information For Resolution (CCIR)</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>100</v>
+      </c>
+      <c r="C28" t="n">
+        <v>100</v>
+      </c>
+      <c r="D28" t="n">
+        <v>100</v>
+      </c>
+      <c r="E28" t="n">
+        <v>100</v>
+      </c>
+      <c r="F28" t="n">
+        <v>100</v>
+      </c>
+      <c r="G28" t="n">
+        <v>100</v>
+      </c>
+      <c r="H28" t="n">
+        <v>100</v>
+      </c>
+      <c r="I28" t="n">
+        <v>100</v>
+      </c>
+      <c r="J28" t="n">
+        <v>100</v>
+      </c>
+      <c r="K28" t="n">
+        <v>92</v>
+      </c>
+      <c r="L28" t="n">
+        <v>100</v>
+      </c>
+      <c r="M28" t="n">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="inlineStr">
+        <is>
+          <t>Identification and Action for Resolution</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>100</v>
+      </c>
+      <c r="C29" t="n">
+        <v>100</v>
+      </c>
+      <c r="D29" t="n">
+        <v>100</v>
+      </c>
+      <c r="E29" t="n">
+        <v>100</v>
+      </c>
+      <c r="F29" t="n">
+        <v>100</v>
+      </c>
+      <c r="G29" t="n">
+        <v>100</v>
+      </c>
+      <c r="H29" t="n">
+        <v>100</v>
+      </c>
+      <c r="I29" t="n">
+        <v>100</v>
+      </c>
+      <c r="J29" t="n">
+        <v>100</v>
+      </c>
+      <c r="K29" t="n">
+        <v>100</v>
+      </c>
+      <c r="L29" t="n">
+        <v>100</v>
+      </c>
+      <c r="M29" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="M30" t="n">
+        <v>99.5</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="M31" t="n">
+        <v>4.97</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="B34" s="1" t="inlineStr">
+        <is>
+          <t>Jan</t>
+        </is>
+      </c>
+      <c r="C34" s="1" t="inlineStr">
+        <is>
+          <t>Feb</t>
+        </is>
+      </c>
+      <c r="D34" s="1" t="inlineStr">
+        <is>
+          <t>Mar</t>
+        </is>
+      </c>
+      <c r="E34" s="1" t="inlineStr">
+        <is>
+          <t>Apr</t>
+        </is>
+      </c>
+      <c r="F34" s="1" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="G34" s="1" t="inlineStr">
+        <is>
+          <t>Jun</t>
+        </is>
+      </c>
+      <c r="H34" s="1" t="inlineStr">
+        <is>
+          <t>Jul</t>
+        </is>
+      </c>
+      <c r="I34" s="1" t="inlineStr">
+        <is>
+          <t>Aug</t>
+        </is>
+      </c>
+      <c r="J34" s="1" t="inlineStr">
+        <is>
+          <t>Sep</t>
+        </is>
+      </c>
+      <c r="K34" s="1" t="inlineStr">
+        <is>
+          <t>Oct</t>
+        </is>
+      </c>
+      <c r="L34" s="1" t="inlineStr">
+        <is>
+          <t>Nov</t>
+        </is>
+      </c>
+      <c r="M34" s="1" t="inlineStr">
+        <is>
+          <t>avg</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="inlineStr">
+        <is>
+          <t>Ownership &amp; Proctiveness (OP)</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>100</v>
+      </c>
+      <c r="C35" t="n">
+        <v>100</v>
+      </c>
+      <c r="D35" t="n">
+        <v>93</v>
+      </c>
+      <c r="E35" t="n">
+        <v>100</v>
+      </c>
+      <c r="F35" t="n">
+        <v>100</v>
+      </c>
+      <c r="G35" t="n">
+        <v>93</v>
+      </c>
+      <c r="H35" t="n">
+        <v>100</v>
+      </c>
+      <c r="I35" t="n">
+        <v>82</v>
+      </c>
+      <c r="J35" t="n">
+        <v>100</v>
+      </c>
+      <c r="K35" t="n">
+        <v>92</v>
+      </c>
+      <c r="L35" t="n">
+        <v>83</v>
+      </c>
+      <c r="M35" t="n">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="M36" t="n">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="M37" t="n">
+        <v>4.7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>